<commit_message>
Try minimal Run with new stuff
</commit_message>
<xml_diff>
--- a/lib/CMRIT2025Leaderboard_Minimal.xlsx
+++ b/lib/CMRIT2025Leaderboard_Minimal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMRIT2025Leaderboard\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE3BBC-B9E0-4218-B2B6-2DBCF441ACCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826F39F-0DBD-4520-8E44-51A86E602218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AB5297C7-CEE9-4FE4-B803-0A47C2167058}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Admn No:</t>
   </si>
@@ -223,6 +223,18 @@
   </si>
   <si>
     <t>charishna</t>
+  </si>
+  <si>
+    <t>21R01A67E6</t>
+  </si>
+  <si>
+    <t>21r01a67e6</t>
+  </si>
+  <si>
+    <t>CMRIT25_21R01A67E6</t>
+  </si>
+  <si>
+    <t>r_21r01a67e6</t>
   </si>
 </sst>
 </file>
@@ -574,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDF3820-1ED2-4581-9EEB-4A4152BC0E3A}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -850,6 +862,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>